<commit_message>
Fix excel file with calculations
</commit_message>
<xml_diff>
--- a/docs/configured_order_calculations.xlsx
+++ b/docs/configured_order_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Virtoway\Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA115DE-78D4-4BA2-99E1-94CEDC8E6DBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE8394E-B1E3-4CAD-B4E9-CCEA5BF5BB5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4FD6E3E5-7644-4892-BB6A-EDDA53C4EA2C}"/>
   </bookViews>
@@ -129,14 +129,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,36 +496,36 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4">
         <f>SUM(I4:I6)</f>
         <v>16.45</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <f>SUM(J4:J6)</f>
         <v>1661.4499999999998</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -551,8 +551,8 @@
         <f>G4*(1+$B$9)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="4">
-        <f>E4*$B$9*C4</f>
+      <c r="I4" s="6">
+        <f>(E4-G4)*C4*$B$9</f>
         <v>14</v>
       </c>
       <c r="J4">
@@ -584,8 +584,8 @@
         <f>G5*(1+$B$9)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="4">
-        <f t="shared" ref="I5:I6" si="0">E5*$B$9*C5</f>
+      <c r="I5" s="6">
+        <f>(E5-G5)*C5*$B$9</f>
         <v>1.6</v>
       </c>
       <c r="J5">
@@ -617,8 +617,8 @@
         <f>G6*(1+$B$9)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="4">
-        <f t="shared" si="0"/>
+      <c r="I6" s="6">
+        <f>(E6-G6)*C6*$B$9</f>
         <v>0.85</v>
       </c>
       <c r="J6">
@@ -630,7 +630,7 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>